<commit_message>
commited by mobasshir again
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -362,7 +362,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -371,26 +371,57 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Websites</t>
+        </is>
+      </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>2019-04-06</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>2019-04-07</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>2019-04-08</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>www.istitutocomprensivotrebisacce.gov.it</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
           <t>www.iscmontegiorgio.it</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>www.istitutocomprensivotrebisacce.gov.it</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="n">
-        <v>-1</v>
-      </c>
-      <c r="C2" t="n">
-        <v>-1</v>
+      <c r="B3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -404,7 +435,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -413,26 +444,57 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Websites</t>
+        </is>
+      </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>2019-04-06</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>2019-04-07</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>2019-04-08</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>www.istitutocomprensivotrebisacce.gov.it</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
           <t>www.iscmontegiorgio.it</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>www.istitutocomprensivotrebisacce.gov.it</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="n">
-        <v>64761</v>
-      </c>
-      <c r="C2" t="n">
-        <v>-1</v>
+      <c r="B3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" t="n">
+        <v>64763</v>
       </c>
     </row>
   </sheetData>
@@ -446,7 +508,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -455,26 +517,57 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Websites</t>
+        </is>
+      </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>2019-04-06</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>2019-04-07</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>2019-04-08</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>www.istitutocomprensivotrebisacce.gov.it</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>26671</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
           <t>www.iscmontegiorgio.it</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>www.istitutocomprensivotrebisacce.gov.it</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="n">
-        <v>105253</v>
-      </c>
-      <c r="C2" t="n">
-        <v>26671</v>
+      <c r="B3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" t="n">
+        <v>105257</v>
       </c>
     </row>
   </sheetData>
@@ -488,7 +581,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -497,26 +590,57 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Websites</t>
+        </is>
+      </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>2019-04-06</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>2019-04-07</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>2019-04-08</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>www.istitutocomprensivotrebisacce.gov.it</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
           <t>www.iscmontegiorgio.it</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>www.istitutocomprensivotrebisacce.gov.it</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="n">
-        <v>-1</v>
-      </c>
-      <c r="C2" t="n">
-        <v>-1</v>
+      <c r="B3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -530,7 +654,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -539,26 +663,57 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Websites</t>
+        </is>
+      </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>2019-04-06</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>2019-04-07</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>2019-04-08</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>www.istitutocomprensivotrebisacce.gov.it</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
           <t>www.iscmontegiorgio.it</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>www.istitutocomprensivotrebisacce.gov.it</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="n">
-        <v>-1</v>
-      </c>
-      <c r="C2" t="n">
-        <v>-1</v>
+      <c r="B3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>